<commit_message>
get data from influx
</commit_message>
<xml_diff>
--- a/log/currency_rate.xlsx
+++ b/log/currency_rate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>2018-06-07 19:46:41</t>
   </si>
@@ -22,30 +22,54 @@
     <t>2018-06-07 19:49:51</t>
   </si>
   <si>
+    <t>2018-06-07 20:00:17</t>
+  </si>
+  <si>
+    <t>2018-06-07 20:10:39</t>
+  </si>
+  <si>
     <t>工商银行</t>
   </si>
   <si>
     <t>640.74</t>
   </si>
   <si>
+    <t>640.71</t>
+  </si>
+  <si>
+    <t>640.69</t>
+  </si>
+  <si>
     <t>农业银行</t>
   </si>
   <si>
     <t>640.28</t>
   </si>
   <si>
+    <t>640.18</t>
+  </si>
+  <si>
     <t>中国银行</t>
   </si>
   <si>
     <t>640.85</t>
   </si>
   <si>
+    <t>640.8</t>
+  </si>
+  <si>
     <t>建设银行</t>
   </si>
   <si>
     <t>640.8000000000001</t>
   </si>
   <si>
+    <t>640.77</t>
+  </si>
+  <si>
+    <t>640.75</t>
+  </si>
+  <si>
     <t>邮储银行</t>
   </si>
   <si>
@@ -58,6 +82,9 @@
     <t>640.86</t>
   </si>
   <si>
+    <t>640.81</t>
+  </si>
+  <si>
     <t>招商银行</t>
   </si>
   <si>
@@ -70,12 +97,15 @@
     <t>640.61</t>
   </si>
   <si>
+    <t>640.58</t>
+  </si>
+  <si>
+    <t>640.56</t>
+  </si>
+  <si>
     <t>兴业银行</t>
   </si>
   <si>
-    <t>640.81</t>
-  </si>
-  <si>
     <t>华夏银行</t>
   </si>
   <si>
@@ -88,6 +118,12 @@
     <t>640.64</t>
   </si>
   <si>
+    <t>640.6</t>
+  </si>
+  <si>
+    <t>640.59</t>
+  </si>
+  <si>
     <t>民生银行</t>
   </si>
   <si>
@@ -100,27 +136,45 @@
     <t>641.18</t>
   </si>
   <si>
+    <t>641.17</t>
+  </si>
+  <si>
+    <t>641.21</t>
+  </si>
+  <si>
     <t>光大银行</t>
   </si>
   <si>
     <t>640.8694</t>
   </si>
   <si>
+    <t>640.8093</t>
+  </si>
+  <si>
     <t>恒丰银行</t>
   </si>
   <si>
+    <t>640.84</t>
+  </si>
+  <si>
+    <t>640.88</t>
+  </si>
+  <si>
     <t>浙商银行</t>
   </si>
   <si>
     <t>641.2</t>
   </si>
   <si>
+    <t>641.19</t>
+  </si>
+  <si>
+    <t>641.23</t>
+  </si>
+  <si>
     <t>渤海银行</t>
   </si>
   <si>
-    <t>640.56</t>
-  </si>
-  <si>
     <t>平安银行</t>
   </si>
   <si>
@@ -148,6 +202,9 @@
     <t>641.05</t>
   </si>
   <si>
+    <t>641.08</t>
+  </si>
+  <si>
     <t>南京银行</t>
   </si>
   <si>
@@ -155,6 +212,12 @@
   </si>
   <si>
     <t>640.94</t>
+  </si>
+  <si>
+    <t>640.89</t>
+  </si>
+  <si>
+    <t>640.83</t>
   </si>
   <si>
     <t>花旗银行</t>
@@ -511,7 +574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,309 +582,477 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing file must be ahead of sorting
</commit_message>
<xml_diff>
--- a/log/currency_rate.xlsx
+++ b/log/currency_rate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="233">
   <si>
     <t>2018-06-07 19:46:41</t>
   </si>
@@ -106,7 +106,7 @@
     <t>2018-06-08 13:18:28</t>
   </si>
   <si>
-    <t>2018-06-08 13:50:56</t>
+    <t>2018-06-08 13:56:36</t>
   </si>
   <si>
     <t>工商银行</t>
@@ -172,228 +172,234 @@
     <t>641.87</t>
   </si>
   <si>
+    <t>641.6</t>
+  </si>
+  <si>
+    <t>农业银行</t>
+  </si>
+  <si>
+    <t>640.28</t>
+  </si>
+  <si>
+    <t>640.18</t>
+  </si>
+  <si>
+    <t>640.98</t>
+  </si>
+  <si>
+    <t>641.18</t>
+  </si>
+  <si>
+    <t>641.28</t>
+  </si>
+  <si>
+    <t>641.36</t>
+  </si>
+  <si>
+    <t>641.43</t>
+  </si>
+  <si>
+    <t>641.53</t>
+  </si>
+  <si>
+    <t>641.48</t>
+  </si>
+  <si>
+    <t>641.73</t>
+  </si>
+  <si>
+    <t>641.68</t>
+  </si>
+  <si>
+    <t>中国银行</t>
+  </si>
+  <si>
+    <t>640.85</t>
+  </si>
+  <si>
+    <t>640.8</t>
+  </si>
+  <si>
+    <t>641.3</t>
+  </si>
+  <si>
+    <t>16291.0</t>
+  </si>
+  <si>
+    <t>641.2</t>
+  </si>
+  <si>
+    <t>641.35</t>
+  </si>
+  <si>
+    <t>641.5</t>
+  </si>
+  <si>
+    <t>641.55</t>
+  </si>
+  <si>
+    <t>641.64</t>
+  </si>
+  <si>
+    <t>641.62</t>
+  </si>
+  <si>
+    <t>641.82</t>
+  </si>
+  <si>
+    <t>Got Wrong</t>
+  </si>
+  <si>
+    <t>641.84</t>
+  </si>
+  <si>
+    <t>建设银行</t>
+  </si>
+  <si>
+    <t>640.8000000000001</t>
+  </si>
+  <si>
+    <t>640.77</t>
+  </si>
+  <si>
+    <t>640.75</t>
+  </si>
+  <si>
+    <t>641.23</t>
+  </si>
+  <si>
     <t>641.45</t>
   </si>
   <si>
-    <t>农业银行</t>
-  </si>
-  <si>
-    <t>640.28</t>
-  </si>
-  <si>
-    <t>640.18</t>
-  </si>
-  <si>
-    <t>640.98</t>
-  </si>
-  <si>
-    <t>641.18</t>
-  </si>
-  <si>
-    <t>641.28</t>
-  </si>
-  <si>
-    <t>641.36</t>
-  </si>
-  <si>
-    <t>641.43</t>
-  </si>
-  <si>
-    <t>641.53</t>
-  </si>
-  <si>
-    <t>641.48</t>
-  </si>
-  <si>
-    <t>641.73</t>
-  </si>
-  <si>
-    <t>641.68</t>
+    <t>641.65</t>
+  </si>
+  <si>
+    <t>641.61</t>
+  </si>
+  <si>
+    <t>641.9100000000001</t>
+  </si>
+  <si>
+    <t>641.8000000000001</t>
+  </si>
+  <si>
+    <t>641.76</t>
+  </si>
+  <si>
+    <t>641.86</t>
+  </si>
+  <si>
+    <t>641.8199999999999</t>
+  </si>
+  <si>
+    <t>641.83</t>
+  </si>
+  <si>
+    <t>641.93</t>
+  </si>
+  <si>
+    <t>641.94</t>
+  </si>
+  <si>
+    <t>641.6800000000001</t>
+  </si>
+  <si>
+    <t>邮储银行</t>
+  </si>
+  <si>
+    <t>640.73</t>
+  </si>
+  <si>
+    <t>640.5</t>
+  </si>
+  <si>
+    <t>641.46</t>
+  </si>
+  <si>
+    <t>641.66</t>
+  </si>
+  <si>
+    <t>交通银行</t>
+  </si>
+  <si>
+    <t>640.86</t>
+  </si>
+  <si>
+    <t>640.81</t>
+  </si>
+  <si>
+    <t>641.44</t>
+  </si>
+  <si>
+    <t>641.58</t>
+  </si>
+  <si>
+    <t>641.72</t>
+  </si>
+  <si>
+    <t>641.7</t>
+  </si>
+  <si>
+    <t>642.</t>
+  </si>
+  <si>
+    <t>641.92</t>
+  </si>
+  <si>
+    <t>641.91</t>
+  </si>
+  <si>
+    <t>641.88</t>
+  </si>
+  <si>
+    <t>641.89</t>
+  </si>
+  <si>
+    <t>招商银行</t>
+  </si>
+  <si>
+    <t>640.95</t>
+  </si>
+  <si>
+    <t>640.6</t>
+  </si>
+  <si>
+    <t>641.75</t>
+  </si>
+  <si>
+    <t>641.9</t>
+  </si>
+  <si>
+    <t>浦发银行</t>
+  </si>
+  <si>
+    <t>640.61</t>
+  </si>
+  <si>
+    <t>640.58</t>
+  </si>
+  <si>
+    <t>640.56</t>
+  </si>
+  <si>
+    <t>640.47</t>
+  </si>
+  <si>
+    <t>641.16</t>
+  </si>
+  <si>
+    <t>641.33</t>
+  </si>
+  <si>
+    <t>641.39</t>
+  </si>
+  <si>
+    <t>641.51</t>
   </si>
   <si>
     <t>641.47</t>
   </si>
   <si>
-    <t>中国银行</t>
-  </si>
-  <si>
-    <t>640.85</t>
-  </si>
-  <si>
-    <t>640.8</t>
-  </si>
-  <si>
-    <t>641.3</t>
-  </si>
-  <si>
-    <t>16291.0</t>
-  </si>
-  <si>
-    <t>641.2</t>
-  </si>
-  <si>
-    <t>641.35</t>
-  </si>
-  <si>
-    <t>641.5</t>
-  </si>
-  <si>
-    <t>641.55</t>
-  </si>
-  <si>
-    <t>641.64</t>
-  </si>
-  <si>
-    <t>641.62</t>
-  </si>
-  <si>
-    <t>641.82</t>
-  </si>
-  <si>
-    <t>Got Wrong</t>
-  </si>
-  <si>
-    <t>641.84</t>
-  </si>
-  <si>
-    <t>建设银行</t>
-  </si>
-  <si>
-    <t>640.8000000000001</t>
-  </si>
-  <si>
-    <t>640.77</t>
-  </si>
-  <si>
-    <t>640.75</t>
-  </si>
-  <si>
-    <t>641.23</t>
-  </si>
-  <si>
-    <t>641.6</t>
-  </si>
-  <si>
-    <t>641.65</t>
-  </si>
-  <si>
-    <t>641.61</t>
-  </si>
-  <si>
-    <t>641.9100000000001</t>
-  </si>
-  <si>
-    <t>641.8000000000001</t>
-  </si>
-  <si>
-    <t>641.76</t>
-  </si>
-  <si>
-    <t>641.86</t>
-  </si>
-  <si>
-    <t>641.8199999999999</t>
-  </si>
-  <si>
-    <t>641.83</t>
-  </si>
-  <si>
-    <t>641.93</t>
-  </si>
-  <si>
-    <t>641.94</t>
-  </si>
-  <si>
-    <t>邮储银行</t>
-  </si>
-  <si>
-    <t>640.73</t>
-  </si>
-  <si>
-    <t>640.5</t>
-  </si>
-  <si>
-    <t>641.46</t>
-  </si>
-  <si>
-    <t>交通银行</t>
-  </si>
-  <si>
-    <t>640.86</t>
-  </si>
-  <si>
-    <t>640.81</t>
-  </si>
-  <si>
-    <t>641.44</t>
-  </si>
-  <si>
-    <t>641.58</t>
-  </si>
-  <si>
-    <t>641.72</t>
-  </si>
-  <si>
-    <t>641.7</t>
-  </si>
-  <si>
-    <t>642.</t>
-  </si>
-  <si>
-    <t>641.92</t>
-  </si>
-  <si>
-    <t>641.91</t>
-  </si>
-  <si>
-    <t>641.88</t>
-  </si>
-  <si>
-    <t>641.89</t>
-  </si>
-  <si>
-    <t>招商银行</t>
-  </si>
-  <si>
-    <t>640.95</t>
-  </si>
-  <si>
-    <t>640.6</t>
-  </si>
-  <si>
-    <t>641.75</t>
-  </si>
-  <si>
-    <t>641.9</t>
-  </si>
-  <si>
-    <t>浦发银行</t>
-  </si>
-  <si>
-    <t>640.61</t>
-  </si>
-  <si>
-    <t>640.58</t>
-  </si>
-  <si>
-    <t>640.56</t>
-  </si>
-  <si>
-    <t>640.47</t>
-  </si>
-  <si>
-    <t>641.16</t>
-  </si>
-  <si>
-    <t>641.33</t>
-  </si>
-  <si>
-    <t>641.39</t>
-  </si>
-  <si>
-    <t>641.51</t>
-  </si>
-  <si>
     <t>641.42</t>
   </si>
   <si>
@@ -463,9 +469,6 @@
     <t>641.7099999999999</t>
   </si>
   <si>
-    <t>641.66</t>
-  </si>
-  <si>
     <t>中信银行</t>
   </si>
   <si>
@@ -514,6 +517,9 @@
     <t>642.26</t>
   </si>
   <si>
+    <t>641.95</t>
+  </si>
+  <si>
     <t>光大银行</t>
   </si>
   <si>
@@ -650,9 +656,6 @@
   </si>
   <si>
     <t>南京银行</t>
-  </si>
-  <si>
-    <t>641.95</t>
   </si>
   <si>
     <t>642.21</t>
@@ -717,12 +720,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -744,13 +754,13 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -1047,11 +1057,11 @@
   </sheetPr>
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:32">
       <c r="B1" t="s">
@@ -1341,122 +1351,122 @@
         <v>63</v>
       </c>
       <c r="AF3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>68</v>
       </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>69</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>70</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
         <v>71</v>
       </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>72</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>73</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" t="s">
         <v>74</v>
       </c>
-      <c r="O4" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>75</v>
       </c>
-      <c r="Q4" t="s">
-        <v>76</v>
-      </c>
       <c r="R4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S4" t="s">
         <v>44</v>
       </c>
       <c r="T4" t="s">
+        <v>76</v>
+      </c>
+      <c r="U4" t="s">
         <v>77</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>78</v>
       </c>
-      <c r="V4" t="s">
-        <v>79</v>
-      </c>
       <c r="W4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Y4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Z4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AA4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AF4" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>82</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -1474,13 +1484,13 @@
         <v>34</v>
       </c>
       <c r="K5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L5" t="s">
         <v>84</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>52</v>
-      </c>
-      <c r="M5" t="s">
-        <v>85</v>
       </c>
       <c r="N5" t="s">
         <v>39</v>
@@ -1489,31 +1499,31 @@
         <v>41</v>
       </c>
       <c r="P5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q5" t="s">
         <v>41</v>
       </c>
       <c r="R5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S5" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>88</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>89</v>
       </c>
-      <c r="U5" t="s">
-        <v>90</v>
-      </c>
       <c r="V5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W5" t="s">
         <v>44</v>
       </c>
       <c r="X5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y5" t="s">
         <v>44</v>
@@ -1525,19 +1535,19 @@
         <v>44</v>
       </c>
       <c r="AB5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC5" t="s">
         <v>92</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>93</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>94</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>95</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:32">
@@ -1617,66 +1627,66 @@
         <v>99</v>
       </c>
       <c r="Z6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AC6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AE6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AF6" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:32">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N7" t="s">
         <v>43</v>
@@ -1685,117 +1695,117 @@
         <v>64</v>
       </c>
       <c r="P7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="U7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Y7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Z7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AA7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AB7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AC7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AD7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AE7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AF7" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
         <v>52</v>
       </c>
-      <c r="L8" t="s">
-        <v>85</v>
-      </c>
       <c r="M8" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="N8" t="s">
         <v>48</v>
       </c>
       <c r="O8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="U8" t="s">
         <v>44</v>
@@ -1807,120 +1817,120 @@
         <v>44</v>
       </c>
       <c r="X8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Y8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Z8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AA8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AB8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AC8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AD8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AE8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AF8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:32">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="P9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q9" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="R9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="S9" t="s">
         <v>63</v>
       </c>
       <c r="T9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="V9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="X9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Y9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Z9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AA9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AB9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AC9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD9" t="s">
         <v>45</v>
@@ -1929,54 +1939,54 @@
         <v>45</v>
       </c>
       <c r="AF9" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:32">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="L10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P10" t="s">
         <v>64</v>
@@ -1988,13 +1998,13 @@
         <v>64</v>
       </c>
       <c r="S10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V10" t="s">
         <v>45</v>
@@ -2018,33 +2028,33 @@
         <v>45</v>
       </c>
       <c r="AC10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AD10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AF10" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:32">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F11" t="s">
         <v>35</v>
@@ -2068,25 +2078,25 @@
         <v>35</v>
       </c>
       <c r="M11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N11" t="s">
         <v>99</v>
       </c>
       <c r="O11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R11" t="s">
         <v>40</v>
       </c>
       <c r="S11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T11" t="s">
         <v>44</v>
@@ -2125,57 +2135,57 @@
         <v>51</v>
       </c>
       <c r="AF11" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:32">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="N12" t="s">
         <v>38</v>
       </c>
       <c r="O12" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="P12" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="Q12" t="s">
         <v>38</v>
@@ -2187,22 +2197,22 @@
         <v>46</v>
       </c>
       <c r="T12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U12" t="s">
         <v>61</v>
       </c>
       <c r="V12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W12" t="s">
         <v>46</v>
       </c>
       <c r="X12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="Y12" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="Z12" t="s">
         <v>46</v>
@@ -2211,30 +2221,30 @@
         <v>46</v>
       </c>
       <c r="AB12" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AC12" t="s">
         <v>45</v>
       </c>
       <c r="AD12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AE12" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AF12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:32">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -2243,28 +2253,28 @@
         <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I13" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="L13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="M13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N13" t="s">
         <v>99</v>
@@ -2276,57 +2286,57 @@
         <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="R13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="S13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="V13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Y13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="Z13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AA13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AB13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="AC13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AD13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AE13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AF13" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
@@ -2335,251 +2345,251 @@
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J14" t="s">
         <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O14" t="s">
+        <v>110</v>
+      </c>
+      <c r="P14" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>93</v>
+      </c>
+      <c r="R14" t="s">
         <v>109</v>
       </c>
-      <c r="P14" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>94</v>
-      </c>
-      <c r="R14" t="s">
-        <v>108</v>
-      </c>
       <c r="S14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="T14" t="s">
+        <v>159</v>
+      </c>
+      <c r="U14" t="s">
+        <v>160</v>
+      </c>
+      <c r="V14" t="s">
+        <v>161</v>
+      </c>
+      <c r="W14" t="s">
+        <v>162</v>
+      </c>
+      <c r="X14" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y14" t="s">
         <v>158</v>
       </c>
-      <c r="U14" t="s">
-        <v>159</v>
-      </c>
-      <c r="V14" t="s">
-        <v>160</v>
-      </c>
-      <c r="W14" t="s">
-        <v>161</v>
-      </c>
-      <c r="X14" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>157</v>
-      </c>
       <c r="Z14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AA14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AB14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AC14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AD14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AE14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AF14" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:32">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="I15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L15" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N15" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="O15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q15" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="R15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="S15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="T15" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="U15" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="V15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="W15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="X15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Y15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Z15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AA15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AB15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AC15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AD15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AE15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF15" t="s">
-        <v>46</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:32">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="I16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K16" t="s">
         <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M16" t="s">
         <v>40</v>
       </c>
       <c r="N16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P16" t="s">
         <v>41</v>
       </c>
       <c r="Q16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R16" t="s">
         <v>42</v>
       </c>
       <c r="S16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="U16" t="s">
         <v>47</v>
@@ -2594,13 +2604,13 @@
         <v>51</v>
       </c>
       <c r="Y16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Z16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB16" t="s">
         <v>49</v>
@@ -2609,30 +2619,30 @@
         <v>44</v>
       </c>
       <c r="AD16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE16" t="s">
         <v>109</v>
       </c>
-      <c r="AE16" t="s">
-        <v>108</v>
-      </c>
       <c r="AF16" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:32">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" t="s">
         <v>58</v>
@@ -2644,22 +2654,22 @@
         <v>58</v>
       </c>
       <c r="I17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J17" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="L17" t="s">
         <v>37</v>
       </c>
       <c r="M17" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="N17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O17" t="s">
         <v>61</v>
@@ -2668,28 +2678,28 @@
         <v>39</v>
       </c>
       <c r="Q17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R17" t="s">
         <v>39</v>
       </c>
       <c r="S17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U17" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="V17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="W17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="X17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Y17" t="s">
         <v>50</v>
@@ -2704,105 +2714,105 @@
         <v>48</v>
       </c>
       <c r="AC17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AD17" t="s">
         <v>51</v>
       </c>
       <c r="AE17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AF17" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:32">
       <c r="A18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" t="s">
+        <v>191</v>
+      </c>
+      <c r="H18" t="s">
+        <v>191</v>
+      </c>
+      <c r="I18" t="s">
+        <v>191</v>
+      </c>
+      <c r="J18" t="s">
+        <v>191</v>
+      </c>
+      <c r="K18" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" t="s">
         <v>188</v>
       </c>
-      <c r="B18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" t="s">
-        <v>189</v>
-      </c>
-      <c r="G18" t="s">
-        <v>189</v>
-      </c>
-      <c r="H18" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" t="s">
-        <v>189</v>
-      </c>
-      <c r="J18" t="s">
-        <v>189</v>
-      </c>
-      <c r="K18" t="s">
-        <v>189</v>
-      </c>
-      <c r="L18" t="s">
-        <v>186</v>
-      </c>
       <c r="M18" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="P18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q18" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="R18" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="S18" t="s">
         <v>47</v>
       </c>
       <c r="T18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U18" t="s">
         <v>43</v>
       </c>
       <c r="V18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W18" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="X18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Y18" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="Z18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA18" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="AB18" t="s">
         <v>41</v>
       </c>
       <c r="AC18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD18" t="s">
         <v>45</v>
@@ -2811,24 +2821,24 @@
         <v>45</v>
       </c>
       <c r="AF18" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:32">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
         <v>98</v>
@@ -2846,25 +2856,25 @@
         <v>56</v>
       </c>
       <c r="K19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="L19" t="s">
         <v>36</v>
       </c>
       <c r="M19" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N19" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="O19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="P19" t="s">
         <v>61</v>
       </c>
       <c r="Q19" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="R19" t="s">
         <v>60</v>
@@ -2873,99 +2883,99 @@
         <v>47</v>
       </c>
       <c r="T19" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="U19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="X19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="Y19" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="Z19" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="AA19" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="AB19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC19" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="AD19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AE19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF19" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:32">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="J20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="K20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M20" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P20" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>74</v>
+      </c>
+      <c r="R20" t="s">
         <v>75</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>75</v>
-      </c>
-      <c r="R20" t="s">
-        <v>76</v>
       </c>
       <c r="S20" t="s">
         <v>39</v>
@@ -2974,57 +2984,57 @@
         <v>39</v>
       </c>
       <c r="U20" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="V20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="W20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="X20" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Y20" t="s">
         <v>51</v>
       </c>
       <c r="Z20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AA20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AB20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AC20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AD20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AE20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AF20" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:32">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F21" t="s">
         <v>34</v>
@@ -3048,10 +3058,10 @@
         <v>34</v>
       </c>
       <c r="M21" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="N21" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="O21" t="s">
         <v>41</v>
@@ -3060,10 +3070,10 @@
         <v>41</v>
       </c>
       <c r="Q21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="R21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="S21" t="s">
         <v>47</v>
@@ -3072,13 +3082,13 @@
         <v>47</v>
       </c>
       <c r="U21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="V21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="W21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="X21" t="s">
         <v>44</v>
@@ -3099,48 +3109,48 @@
         <v>44</v>
       </c>
       <c r="AD21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AF21" t="s">
-        <v>178</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:32">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="J22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="K22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L22" t="s">
         <v>60</v>
@@ -3149,10 +3159,10 @@
         <v>40</v>
       </c>
       <c r="N22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="O22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="P22" t="s">
         <v>39</v>
@@ -3161,164 +3171,164 @@
         <v>41</v>
       </c>
       <c r="R22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U22" t="s">
         <v>63</v>
       </c>
       <c r="V22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="W22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="X22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Y22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Z22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AA22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AC22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AD22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AE22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF22" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:32">
       <c r="A23" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="I23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="J23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="L23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="M23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="N23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="O23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="P23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="Q23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="R23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="S23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="T23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="U23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="V23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="W23" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="X23" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="Y23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="Z23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AA23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AB23" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="AC23" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AD23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AE23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AF23" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:32">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
         <v>58</v>
@@ -3339,105 +3349,105 @@
         <v>58</v>
       </c>
       <c r="L24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N24" t="s">
+        <v>93</v>
+      </c>
+      <c r="O24" t="s">
+        <v>93</v>
+      </c>
+      <c r="P24" t="s">
         <v>94</v>
       </c>
-      <c r="O24" t="s">
+      <c r="Q24" t="s">
+        <v>167</v>
+      </c>
+      <c r="R24" t="s">
         <v>94</v>
       </c>
-      <c r="P24" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>212</v>
-      </c>
-      <c r="R24" t="s">
-        <v>95</v>
-      </c>
       <c r="S24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="T24" t="s">
+        <v>215</v>
+      </c>
+      <c r="U24" t="s">
+        <v>155</v>
+      </c>
+      <c r="V24" t="s">
+        <v>216</v>
+      </c>
+      <c r="W24" t="s">
+        <v>217</v>
+      </c>
+      <c r="X24" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y24" t="s">
         <v>214</v>
       </c>
-      <c r="U24" t="s">
-        <v>154</v>
-      </c>
-      <c r="V24" t="s">
-        <v>215</v>
-      </c>
-      <c r="W24" t="s">
-        <v>216</v>
-      </c>
-      <c r="X24" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>213</v>
-      </c>
       <c r="Z24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AA24" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AB24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AC24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AD24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AE24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AF24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:32">
       <c r="A25" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C25" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D25" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F25" t="s">
         <v>64</v>
       </c>
       <c r="G25" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H25" t="s">
         <v>61</v>
       </c>
       <c r="I25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J25" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K25" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="L25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M25" t="s">
         <v>41</v>
@@ -3458,343 +3468,344 @@
         <v>45</v>
       </c>
       <c r="S25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="T25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U25" t="s">
         <v>51</v>
       </c>
       <c r="V25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="W25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="X25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Y25" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="Z25" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="AA25" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="AB25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AC25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AD25" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AE25" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AF25" t="s">
-        <v>212</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:32">
       <c r="A26" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="J26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Q26" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="R26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="S26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="T26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="U26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="V26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="W26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="X26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="Y26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="Z26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AA26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AB26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AC26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AD26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AE26" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="AF26" t="s">
-        <v>208</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:32">
       <c r="A27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="N27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="O27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Q27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="S27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="T27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="U27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="V27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="W27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="X27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Y27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Z27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AA27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AB27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AC27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AD27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AE27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AF27" t="s">
-        <v>164</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:32">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C28" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="J28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="L28" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="M28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="O28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="P28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="R28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="T28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="U28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="V28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="W28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="X28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Y28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Z28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AA28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AB28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AC28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AD28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AE28" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AF28" t="s">
-        <v>229</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>